<commit_message>
recorriendo datos del excel v01
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/DataDriven.xlsx
+++ b/src/main/resources/Data/DataDriven.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matias.rojas\IdeaProjects\EjerciciosAutomatizacion\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85C977A-69E1-499F-B2A6-D61F3391252D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2937D09-C447-4862-AB00-877CF2F56010}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{C46FAF6A-F493-4035-8392-1F2F68894BAB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t>Caso de Prueba</t>
-  </si>
-  <si>
     <t>ATC05</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Internet</t>
+  </si>
+  <si>
+    <t>TestCase</t>
   </si>
 </sst>
 </file>
@@ -437,9 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9501186-1ED4-4B6E-997F-EFCD42B67C8B}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -453,77 +451,77 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>